<commit_message>
Estilizando e dando toques finais
</commit_message>
<xml_diff>
--- a/spreadsheets/gabarito_modelo.xlsx
+++ b/spreadsheets/gabarito_modelo.xlsx
@@ -5,10 +5,10 @@
   <workbookPr hidePivotFieldList="1" defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\vinim\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\vinim\Documents\Projects GitHub\Automated-Multiple-Choice-Exam-Grading-System\spreadsheets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B394A988-2D98-4006-A93F-683BDB1807C6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2B99C7D2-1156-479E-8575-743AE99B6361}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{D3219A13-647C-4E61-9BEB-CAC4A9BE4460}"/>
   </bookViews>
@@ -36,18 +36,9 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="14">
   <si>
     <t>NUMERO DA QUESTÃO</t>
-  </si>
-  <si>
-    <t>01</t>
-  </si>
-  <si>
-    <t>02</t>
-  </si>
-  <si>
-    <t>03</t>
   </si>
   <si>
     <t>MATÉRIA</t>
@@ -78,6 +69,15 @@
   </si>
   <si>
     <t>1A 1 BIMESTRE 1 DIA</t>
+  </si>
+  <si>
+    <t>1</t>
+  </si>
+  <si>
+    <t>2</t>
+  </si>
+  <si>
+    <t>3</t>
   </si>
 </sst>
 </file>
@@ -158,7 +158,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="3">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -168,25 +168,16 @@
     </border>
     <border>
       <left style="thin">
-        <color indexed="64"/>
+        <color theme="2" tint="-0.749992370372631"/>
       </left>
       <right style="thin">
-        <color indexed="64"/>
+        <color theme="2" tint="-0.749992370372631"/>
       </right>
       <top style="thin">
-        <color indexed="64"/>
+        <color theme="2" tint="-0.749992370372631"/>
       </top>
       <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="thin">
-        <color indexed="64"/>
+        <color theme="2" tint="-0.749992370372631"/>
       </bottom>
       <diagonal/>
     </border>
@@ -194,9 +185,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="49" fontId="3" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -214,12 +208,651 @@
     <xf numFmtId="49" fontId="6" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="7">
+  <dxfs count="40">
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="3" tint="0.89996032593768116"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.14996795556505021"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="4" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <fgColor theme="5" tint="-0.24994659260841701"/>
+          <bgColor rgb="FFFFFF66"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <fgColor theme="1"/>
+          <bgColor theme="3" tint="0.499984740745262"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF7C80"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="2" tint="-9.9948118533890809E-2"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.14996795556505021"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="4" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <fgColor theme="5" tint="-0.24994659260841701"/>
+          <bgColor rgb="FFFFFF66"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <fgColor theme="1"/>
+          <bgColor theme="3" tint="0.499984740745262"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF7C80"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="2" tint="-9.9948118533890809E-2"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.14996795556505021"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="4" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <fgColor theme="5" tint="-0.24994659260841701"/>
+          <bgColor rgb="FFFFFF66"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <fgColor theme="1"/>
+          <bgColor theme="3" tint="0.499984740745262"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF7C80"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="2" tint="-9.9948118533890809E-2"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.14996795556505021"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="4" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <fgColor theme="5" tint="-0.24994659260841701"/>
+          <bgColor rgb="FFFFFF66"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <fgColor theme="1"/>
+          <bgColor theme="3" tint="0.499984740745262"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF7C80"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.14996795556505021"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="4" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <fgColor theme="5" tint="-0.24994659260841701"/>
+          <bgColor rgb="FFFFFF66"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF7C80"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <fill>
         <patternFill>
@@ -289,7 +922,7 @@
   </dxfs>
   <tableStyles count="5" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16">
     <tableStyle name="Estilo de Tabela 1" pivot="0" count="1" xr9:uid="{229E56E9-8E29-4486-80B2-134F3B256510}">
-      <tableStyleElement type="wholeTable" dxfId="6"/>
+      <tableStyleElement type="wholeTable" dxfId="39"/>
     </tableStyle>
     <tableStyle name="Estilo de Tabela Dinâmica 1" table="0" count="0" xr9:uid="{0E0CDC08-B0E2-4A8E-80D0-F74B60C9F1F5}"/>
     <tableStyle name="Estilo de Tabela Dinâmica 2" table="0" count="0" xr9:uid="{95A0F887-2E86-4EE2-ABCE-F2261183225F}"/>
@@ -624,10 +1257,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CF8CBFC7-BDF7-4025-9601-D1585C9FCE9A}">
-  <dimension ref="A1:H6"/>
+  <dimension ref="A1:U16"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="I4" sqref="I4"/>
+      <selection activeCell="R7" sqref="R7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -696,98 +1329,288 @@
     <col min="121" max="121" width="10" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="21" x14ac:dyDescent="0.4">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:21" ht="21" x14ac:dyDescent="0.4">
+      <c r="A1" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="B1" s="4"/>
+      <c r="C1" s="4"/>
+      <c r="D1" s="4"/>
+      <c r="E1" s="2"/>
+      <c r="F1" s="2"/>
+    </row>
+    <row r="2" spans="1:21" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A2" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="C2" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="D2" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="B1" s="1"/>
-      <c r="C1" s="1"/>
-      <c r="D1" s="1"/>
+      <c r="E2" s="2"/>
+      <c r="F2" s="2"/>
     </row>
-    <row r="2" spans="1:8" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A2" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="B2" s="3" t="s">
+    <row r="3" spans="1:21" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A3" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="3" t="s">
+      <c r="B3" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="C3" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="D3" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="E3" s="2"/>
+      <c r="F3" s="2"/>
+    </row>
+    <row r="4" spans="1:21" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A4" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="D2" s="3" t="s">
+      <c r="B4" s="8" t="s">
         <v>3</v>
       </c>
+      <c r="C4" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="D4" s="8" t="s">
+        <v>5</v>
+      </c>
+      <c r="E4" s="2"/>
+      <c r="F4" s="2"/>
     </row>
-    <row r="3" spans="1:8" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A3" s="4" t="s">
+    <row r="5" spans="1:21" ht="15" x14ac:dyDescent="0.3">
+      <c r="A5" s="9" t="s">
+        <v>7</v>
+      </c>
+      <c r="B5" s="8" t="s">
+        <v>3</v>
+      </c>
+      <c r="C5" s="8" t="s">
+        <v>3</v>
+      </c>
+      <c r="D5" s="8"/>
+      <c r="E5" s="2"/>
+      <c r="F5" s="2"/>
+    </row>
+    <row r="6" spans="1:21" ht="15" x14ac:dyDescent="0.3">
+      <c r="A6" s="9" t="s">
+        <v>7</v>
+      </c>
+      <c r="B6" s="8" t="s">
         <v>4</v>
       </c>
-      <c r="B3" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="C3" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="D3" s="3" t="s">
-        <v>9</v>
-      </c>
+      <c r="C6" s="8"/>
+      <c r="D6" s="8" t="s">
+        <v>5</v>
+      </c>
+      <c r="E6" s="2"/>
+      <c r="F6" s="2"/>
+      <c r="H6" s="1"/>
     </row>
-    <row r="4" spans="1:8" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A4" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="B4" s="5" t="s">
-        <v>6</v>
-      </c>
-      <c r="C4" s="5" t="s">
-        <v>7</v>
-      </c>
-      <c r="D4" s="5" t="s">
-        <v>8</v>
-      </c>
+    <row r="7" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="E7" s="2"/>
+      <c r="F7" s="2"/>
+      <c r="H7" s="2"/>
+      <c r="I7" s="2"/>
+      <c r="J7" s="2"/>
+      <c r="K7" s="2"/>
+      <c r="L7" s="2"/>
+      <c r="M7" s="2"/>
+      <c r="N7" s="2"/>
+      <c r="O7" s="2"/>
+      <c r="P7" s="2"/>
+      <c r="Q7" s="2"/>
+      <c r="R7" s="3"/>
+      <c r="S7" s="2"/>
+      <c r="T7" s="2"/>
+      <c r="U7" s="2"/>
     </row>
-    <row r="5" spans="1:8" ht="15" x14ac:dyDescent="0.3">
-      <c r="A5" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="B5" s="5" t="s">
-        <v>6</v>
-      </c>
-      <c r="C5" s="5" t="s">
-        <v>6</v>
-      </c>
-      <c r="D5" s="5"/>
+    <row r="8" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="H8" s="2"/>
+      <c r="I8" s="2"/>
+      <c r="J8" s="2"/>
+      <c r="K8" s="2"/>
+      <c r="L8" s="2"/>
+      <c r="M8" s="2"/>
+      <c r="N8" s="2"/>
+      <c r="O8" s="2"/>
+      <c r="P8" s="2"/>
+      <c r="Q8" s="2"/>
+      <c r="R8" s="2"/>
+      <c r="S8" s="2"/>
+      <c r="T8" s="2"/>
+      <c r="U8" s="2"/>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="H6" s="7"/>
+    <row r="9" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="E9" s="2"/>
+      <c r="H9" s="2"/>
+      <c r="I9" s="2"/>
+      <c r="J9" s="2"/>
+      <c r="K9" s="2"/>
+      <c r="L9" s="2"/>
+      <c r="M9" s="2"/>
+      <c r="N9" s="2"/>
+      <c r="O9" s="2"/>
+      <c r="P9" s="2"/>
+      <c r="Q9" s="2"/>
+      <c r="R9" s="2"/>
+      <c r="S9" s="2"/>
+      <c r="T9" s="2"/>
+      <c r="U9" s="2"/>
+    </row>
+    <row r="10" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="H10" s="2"/>
+      <c r="I10" s="2"/>
+      <c r="J10" s="2"/>
+      <c r="K10" s="2"/>
+      <c r="L10" s="2"/>
+      <c r="M10" s="2"/>
+      <c r="N10" s="2"/>
+      <c r="O10" s="2"/>
+      <c r="P10" s="2"/>
+      <c r="Q10" s="2"/>
+      <c r="R10" s="2"/>
+      <c r="S10" s="2"/>
+      <c r="T10" s="2"/>
+      <c r="U10" s="2"/>
+    </row>
+    <row r="11" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="H11" s="2"/>
+      <c r="I11" s="2"/>
+      <c r="J11" s="2"/>
+      <c r="K11" s="2"/>
+      <c r="L11" s="2"/>
+      <c r="M11" s="2"/>
+      <c r="N11" s="2"/>
+      <c r="O11" s="2"/>
+      <c r="P11" s="2"/>
+      <c r="Q11" s="2"/>
+      <c r="R11" s="2"/>
+      <c r="S11" s="2"/>
+      <c r="T11" s="2"/>
+      <c r="U11" s="2"/>
+    </row>
+    <row r="12" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="H12" s="2"/>
+      <c r="I12" s="2"/>
+      <c r="J12" s="2"/>
+      <c r="K12" s="2"/>
+      <c r="L12" s="2"/>
+      <c r="M12" s="2"/>
+      <c r="N12" s="2"/>
+      <c r="O12" s="2"/>
+      <c r="P12" s="2"/>
+      <c r="Q12" s="2"/>
+      <c r="R12" s="2"/>
+      <c r="S12" s="2"/>
+      <c r="T12" s="2"/>
+      <c r="U12" s="2"/>
+    </row>
+    <row r="13" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="H13" s="2"/>
+      <c r="I13" s="2"/>
+      <c r="J13" s="2"/>
+      <c r="K13" s="2"/>
+      <c r="L13" s="2"/>
+      <c r="M13" s="2"/>
+      <c r="N13" s="2"/>
+      <c r="O13" s="2"/>
+      <c r="P13" s="2"/>
+      <c r="Q13" s="2"/>
+      <c r="R13" s="2"/>
+      <c r="S13" s="2"/>
+      <c r="T13" s="2"/>
+      <c r="U13" s="2"/>
+    </row>
+    <row r="14" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="H14" s="2"/>
+      <c r="I14" s="2"/>
+      <c r="J14" s="2"/>
+      <c r="K14" s="2"/>
+      <c r="L14" s="2"/>
+      <c r="M14" s="2"/>
+      <c r="N14" s="2"/>
+      <c r="O14" s="2"/>
+      <c r="P14" s="2"/>
+      <c r="Q14" s="2"/>
+      <c r="R14" s="2"/>
+      <c r="S14" s="2"/>
+      <c r="T14" s="2"/>
+      <c r="U14" s="2"/>
+    </row>
+    <row r="15" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="H15" s="2"/>
+      <c r="I15" s="2"/>
+      <c r="J15" s="2"/>
+      <c r="K15" s="2"/>
+      <c r="L15" s="2"/>
+      <c r="M15" s="2"/>
+      <c r="N15" s="2"/>
+      <c r="O15" s="2"/>
+      <c r="P15" s="2"/>
+      <c r="Q15" s="2"/>
+      <c r="R15" s="2"/>
+      <c r="S15" s="2"/>
+      <c r="T15" s="2"/>
+      <c r="U15" s="2"/>
+    </row>
+    <row r="16" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="H16" s="2"/>
+      <c r="I16" s="2"/>
+      <c r="J16" s="2"/>
+      <c r="K16" s="2"/>
+      <c r="L16" s="2"/>
+      <c r="M16" s="2"/>
+      <c r="N16" s="2"/>
+      <c r="O16" s="2"/>
+      <c r="P16" s="2"/>
+      <c r="Q16" s="2"/>
+      <c r="R16" s="2"/>
+      <c r="S16" s="2"/>
+      <c r="T16" s="2"/>
+      <c r="U16" s="2"/>
     </row>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="A1:D1"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
-  <conditionalFormatting sqref="A3 A4:D5">
-    <cfRule type="expression" dxfId="5" priority="28">
+  <conditionalFormatting sqref="A3 A4:D6">
+    <cfRule type="expression" dxfId="6" priority="30">
       <formula>AND((A3=A$4), (LEN(A3)&lt;2))</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="4" priority="29">
+    <cfRule type="expression" dxfId="5" priority="31">
       <formula>AND((A3&lt;&gt;A$4), (LEN(A3)&lt;2))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A2:D2">
-    <cfRule type="expression" dxfId="3" priority="25">
+    <cfRule type="expression" dxfId="4" priority="27">
       <formula>ROW()=2</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A3:D5">
-    <cfRule type="expression" dxfId="2" priority="24">
+  <conditionalFormatting sqref="A3:D6">
+    <cfRule type="expression" dxfId="3" priority="26">
       <formula>ROW()=4</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="1" priority="26">
+    <cfRule type="expression" dxfId="2" priority="28">
       <formula>$A3="MATÉRIA"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="0" priority="27">
+    <cfRule type="expression" dxfId="1" priority="29">
       <formula>AND((A3=""), (LEN(A3)&lt;2))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A5:A6">
+    <cfRule type="expression" dxfId="0" priority="2">
+      <formula>MOD(ROW($A5),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>

</xml_diff>